<commit_message>
added excel and some option pricing code
</commit_message>
<xml_diff>
--- a/excel/listed_price1.xlsx
+++ b/excel/listed_price1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stirlitz/ncGitHub/llm_options_app1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stirlitz/ncGitHub/llm_options_app1/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AD08FC-ACCC-A14C-AC4F-13F791786A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF62B21-6C08-5F46-858C-38AFC54F1435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4360" yWindow="680" windowWidth="30200" windowHeight="19760" xr2:uid="{263D9CF6-C2BD-4D47-ACEB-BB9BA3F75454}"/>
   </bookViews>
@@ -636,7 +636,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -667,8 +667,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -676,15 +682,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -696,6 +741,11 @@
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,24 +832,24 @@
     <v t="s">Vol</v>
     <v t="s">borrow</v>
     <v>0</v>
-    <v>1000000</v>
+    <v>100000</v>
     <v t="r">6</v>
     <v>180</v>
     <v>183.22</v>
     <v t="s">P</v>
     <v t="s">A</v>
-    <v>1.2444444444444445</v>
+    <v>1.3888888888888888E-2</v>
     <v t="r">0</v>
     <v>0.4375</v>
     <v>0</v>
     <v>1</v>
-    <v>1000000</v>
+    <v>100000</v>
     <v t="r">6</v>
     <v>180</v>
     <v>183.22</v>
     <v t="s">C</v>
     <v t="s">A</v>
-    <v>1.2444444444444445</v>
+    <v>1.3888888888888888E-2</v>
     <v t="r">0</v>
     <v>0.4375</v>
     <v>0</v>
@@ -856,29 +906,29 @@
     <v t="s">Rho</v>
     <v t="s">Rho01</v>
     <v>0</v>
-    <v>1000000</v>
+    <v>100000</v>
     <v t="r">6</v>
     <v>180</v>
     <v>183.22</v>
     <v t="s">P</v>
     <v t="s">...</v>
-    <v>764898.46278708207</v>
-    <v>-10879499.13942232</v>
-    <v>-29806.846957321424</v>
-    <v>-91384913.508427694</v>
-    <v>-9138.4913508427708</v>
+    <v>8023.3992552592099</v>
+    <v>-12423513.905567631</v>
+    <v>-34037.024398815433</v>
+    <v>-86267.210155810404</v>
+    <v>-8.6267210155810403</v>
     <v>1</v>
-    <v>1000000</v>
+    <v>100000</v>
     <v t="r">6</v>
     <v>180</v>
     <v>183.22</v>
     <v t="s">C</v>
     <v t="s">...</v>
-    <v>760828.07561082428</v>
-    <v>-16110673.891427141</v>
-    <v>-44138.832579252441</v>
-    <v>96956978.77582176</v>
-    <v>9695.6978775821772</v>
+    <v>8020.1967944819153</v>
+    <v>-13031273.298313977</v>
+    <v>-35702.118625517745</v>
+    <v>156949.96482373824</v>
+    <v>15.694996482373824</v>
   </a>
   <a r="3" c="5">
     <v t="s"/>
@@ -887,15 +937,15 @@
     <v t="s">Gamma</v>
     <v t="s">Vega01</v>
     <v>0</v>
-    <v>29.871165597845863</v>
-    <v>-0.36994905378514381</v>
-    <v>4448.8290148558272</v>
-    <v>764898.46278708207</v>
+    <v>2.3095554082585976</v>
+    <v>-0.35305563284214747</v>
+    <v>3938.8817428978164</v>
+    <v>8023.3992552592099</v>
     <v>1</v>
-    <v>39.952099164325155</v>
-    <v>0.64378101699318313</v>
-    <v>4163.3692204800382</v>
-    <v>760828.07561082428</v>
+    <v>5.6151629774481515</v>
+    <v>0.64733544856512815</v>
+    <v>3931.9723866686077</v>
+    <v>8020.1967944819153</v>
   </a>
 </arrayData>
 </file>
@@ -935,7 +985,7 @@
     <v>1</v>
   </rv>
   <rv s="0">
-    <fb>46403</fb>
+    <fb>45953</fb>
     <v>2</v>
   </rv>
   <rv s="2">
@@ -949,11 +999,11 @@
   <rv s="1">
     <v>&lt;class 'pandas.core.frame.DataFrame'&gt;</v>
     <v>DataFrame</v>
-    <v xml:space="preserve">      mult Expiration  Strike    Spot CP EA      Texp Vol Override     Vol  \
-0  1000000 2027-01-16     180  183.22  P  A  1.244444         None  0.4375   
-1  1000000 2027-01-16     180  183.22  C  A  1.244444         None  0.4375   
+    <v xml:space="preserve">     mult Expiration  Strike    Spot CP EA      Texp Vol Override     Vol  \
+0  100000 2025-10-23     180  183.22  P  A  0.013889         None  0.4375   
+1  100000 2025-10-23     180  183.22  C  A  0.013889         None  0.4375   
    borrow  
-0    ...</v>
+0       ...</v>
     <v>8</v>
     <v>1</v>
   </rv>
@@ -1034,10 +1084,10 @@
   <rv s="1">
     <v>&lt;class 'pandas.core.frame.DataFrame'&gt;</v>
     <v>DataFrame</v>
-    <v xml:space="preserve">      mult expiration  strike    spot cp ea      texp vol override     vol  \
-0  1000000 2027-01-16     180  183.22  P  A  1.244444         None  0.4375   
-1  1000000 2027-01-16     180  183.22  C  A  1.244444         None  0.4375   
-   borrow  ...   ...</v>
+    <v xml:space="preserve">     mult expiration  strike    spot cp ea      texp vol override     vol  \
+0  100000 2025-10-23     180  183.22  P  A  0.013889         None  0.4375   
+1  100000 2025-10-23     180  183.22  C  A  0.013889         None  0.4375   
+   borrow  ...     d...</v>
     <v>24</v>
     <v>1</v>
   </rv>
@@ -1052,9 +1102,9 @@
   <rv s="1">
     <v>&lt;class 'pandas.core.frame.DataFrame'&gt;</v>
     <v>DataFrame</v>
-    <v xml:space="preserve">       price     delta        Gamma         Vega01
-0  29.871166 -0.369949  4448.829015  764898.462787
-1  39.952099  0.643781  4163.369220  760828.075611</v>
+    <v xml:space="preserve">      price     delta        Gamma       Vega01
+0  2.309555 -0.353056  3938.881743  8023.399255
+1  5.615163  0.647335  3931.972387  8020.196794</v>
     <v>27</v>
     <v>1</v>
   </rv>
@@ -1517,7 +1567,7 @@
   <dimension ref="A1:AD58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1533,7 +1583,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="1" cm="1" vm="1">
@@ -1543,7 +1593,7 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="1" cm="1" vm="1">
@@ -1552,7 +1602,7 @@
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="1" cm="1" vm="1">
@@ -1561,25 +1611,26 @@
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="W5" s="1" t="s">
+      <c r="W5" s="14" t="s">
         <v>6</v>
       </c>
+      <c r="X5" s="14"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="W6" s="1" t="s">
+      <c r="G6" s="4"/>
+      <c r="W6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="X6" s="14" t="s">
         <v>31</v>
       </c>
       <c r="Y6" s="1" cm="1">
@@ -1603,23 +1654,23 @@
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <v>45969</v>
       </c>
-      <c r="W7" s="3">
+      <c r="W7" s="17">
         <f>G7</f>
         <v>45969</v>
       </c>
-      <c r="X7" s="1">
+      <c r="X7" s="18">
         <f>G9</f>
         <v>0.01</v>
       </c>
@@ -1643,98 +1694,98 @@
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>183.22</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>4</v>
       </c>
       <c r="V8" s="1">
         <v>1</v>
       </c>
-      <c r="W8" s="3">
+      <c r="W8" s="15">
         <f t="shared" ref="W8:W28" si="0">WORKDAY(EDATE($W$7,12/$G$8*V8)-1,1)</f>
         <v>46062</v>
       </c>
-      <c r="X8" s="1">
+      <c r="X8" s="16">
         <f>X7+IF(MOD(V8,4)=0,$G$10,0)</f>
         <v>0.01</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="11">
         <v>0</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>0.01</v>
       </c>
       <c r="V9" s="1">
         <f>V8+1</f>
         <v>2</v>
       </c>
-      <c r="W9" s="3">
+      <c r="W9" s="15">
         <f t="shared" si="0"/>
         <v>46150</v>
       </c>
-      <c r="X9" s="1">
+      <c r="X9" s="16">
         <f t="shared" ref="X9:X19" si="1">X8+IF(MOD(V9,4)=0,$G$10,0)</f>
         <v>0.01</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="7">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>0</v>
       </c>
       <c r="V10" s="1">
         <f t="shared" ref="V10:V28" si="2">V9+1</f>
         <v>3</v>
       </c>
-      <c r="W10" s="3">
+      <c r="W10" s="15">
         <f t="shared" si="0"/>
         <v>46244</v>
       </c>
-      <c r="X10" s="1">
+      <c r="X10" s="16">
         <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>45948</v>
       </c>
       <c r="V11" s="1">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="W11" s="3">
+      <c r="W11" s="15">
         <f t="shared" si="0"/>
         <v>46335</v>
       </c>
-      <c r="X11" s="1">
+      <c r="X11" s="16">
         <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
@@ -1744,11 +1795,11 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="W12" s="3">
+      <c r="W12" s="15">
         <f t="shared" si="0"/>
         <v>46426</v>
       </c>
-      <c r="X12" s="1">
+      <c r="X12" s="16">
         <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
@@ -1758,11 +1809,11 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="W13" s="3">
+      <c r="W13" s="15">
         <f t="shared" si="0"/>
         <v>46517</v>
       </c>
-      <c r="X13" s="1">
+      <c r="X13" s="16">
         <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
@@ -1772,11 +1823,11 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="W14" s="3">
+      <c r="W14" s="15">
         <f t="shared" si="0"/>
         <v>46608</v>
       </c>
-      <c r="X14" s="1">
+      <c r="X14" s="16">
         <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
@@ -1786,191 +1837,191 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="W15" s="3">
+      <c r="W15" s="15">
         <f t="shared" si="0"/>
         <v>46699</v>
       </c>
-      <c r="X15" s="1">
+      <c r="X15" s="16">
         <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="J16" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="K16" s="6" t="s">
+      <c r="K16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="M16" s="10" t="str" cm="1">
+      <c r="M16" s="9" t="str" cm="1">
         <f t="array" ref="M16:Q18">_FV(C53,"arrayPreview")</f>
         <v/>
       </c>
-      <c r="N16" s="10" t="str">
+      <c r="N16" s="9" t="str">
         <v>price</v>
       </c>
-      <c r="O16" s="10" t="str">
+      <c r="O16" s="9" t="str">
         <v>delta</v>
       </c>
-      <c r="P16" s="10" t="str">
+      <c r="P16" s="9" t="str">
         <v>Gamma</v>
       </c>
-      <c r="Q16" s="10" t="str">
+      <c r="Q16" s="9" t="str">
         <v>Vega01</v>
       </c>
       <c r="V16" s="1">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="W16" s="3">
+      <c r="W16" s="15">
         <f t="shared" si="0"/>
         <v>46791</v>
       </c>
-      <c r="X16" s="1">
+      <c r="X16" s="16">
         <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
     </row>
     <row r="17" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B17" s="11">
-        <v>1000000</v>
-      </c>
-      <c r="C17" s="9">
-        <v>46403</v>
-      </c>
-      <c r="D17" s="7">
+      <c r="B17" s="10">
+        <v>100000</v>
+      </c>
+      <c r="C17" s="8">
+        <v>45953</v>
+      </c>
+      <c r="D17" s="6">
         <v>180</v>
       </c>
       <c r="E17" s="1">
         <f>$D$8</f>
         <v>183.22</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="6" t="s">
         <v>5</v>
       </c>
       <c r="H17" s="1">
         <f>YEARFRAC($D$11,C17)</f>
-        <v>1.2444444444444445</v>
-      </c>
-      <c r="I17" s="13"/>
-      <c r="J17" s="4">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="I17" s="12"/>
+      <c r="J17" s="3">
         <f>IF(ISBLANK(I17),$G$21+10*$G$22*LN(D17/E17)/SQRT(H17),I17)</f>
         <v>0.4375</v>
       </c>
-      <c r="K17" s="14">
+      <c r="K17" s="13">
         <v>0</v>
       </c>
       <c r="M17" s="1">
         <v>0</v>
       </c>
       <c r="N17" s="1">
-        <v>29.871165597845863</v>
+        <v>2.3095554082585976</v>
       </c>
       <c r="O17" s="1">
-        <v>-0.36994905378514381</v>
+        <v>-0.35305563284214747</v>
       </c>
       <c r="P17" s="1">
-        <v>4448.8290148558272</v>
+        <v>3938.8817428978164</v>
       </c>
       <c r="Q17" s="1">
-        <v>764898.46278708207</v>
+        <v>8023.3992552592099</v>
       </c>
       <c r="V17" s="1">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="W17" s="3">
+      <c r="W17" s="15">
         <f t="shared" si="0"/>
         <v>46881</v>
       </c>
-      <c r="X17" s="1">
+      <c r="X17" s="16">
         <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
     </row>
     <row r="18" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B18" s="11">
-        <v>1000000</v>
-      </c>
-      <c r="C18" s="9">
-        <v>46403</v>
-      </c>
-      <c r="D18" s="7">
+      <c r="B18" s="10">
+        <v>100000</v>
+      </c>
+      <c r="C18" s="8">
+        <v>45953</v>
+      </c>
+      <c r="D18" s="6">
         <v>180</v>
       </c>
       <c r="E18" s="1">
         <f>$D$8</f>
         <v>183.22</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="6" t="s">
         <v>5</v>
       </c>
       <c r="H18" s="1">
         <f>YEARFRAC($D$11,C18)</f>
-        <v>1.2444444444444445</v>
-      </c>
-      <c r="I18" s="13"/>
-      <c r="J18" s="4">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="I18" s="12"/>
+      <c r="J18" s="3">
         <f>IF(ISBLANK(I18),$G$21+10*$G$22*LN(D18/E18)/SQRT(H18),I18)</f>
         <v>0.4375</v>
       </c>
-      <c r="K18" s="14">
+      <c r="K18" s="13">
         <v>0</v>
       </c>
       <c r="M18" s="1">
         <v>1</v>
       </c>
       <c r="N18" s="1">
-        <v>39.952099164325155</v>
+        <v>5.6151629774481515</v>
       </c>
       <c r="O18" s="1">
-        <v>0.64378101699318313</v>
+        <v>0.64733544856512815</v>
       </c>
       <c r="P18" s="1">
-        <v>4163.3692204800382</v>
+        <v>3931.9723866686077</v>
       </c>
       <c r="Q18" s="1">
-        <v>760828.07561082428</v>
+        <v>8020.1967944819153</v>
       </c>
       <c r="V18" s="1">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="W18" s="3">
+      <c r="W18" s="15">
         <f t="shared" si="0"/>
         <v>46973</v>
       </c>
-      <c r="X18" s="1">
+      <c r="X18" s="16">
         <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
@@ -1983,11 +2034,11 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="W19" s="3">
+      <c r="W19" s="15">
         <f t="shared" si="0"/>
         <v>47065</v>
       </c>
-      <c r="X19" s="1">
+      <c r="X19" s="16">
         <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
@@ -1997,51 +2048,51 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="W20" s="3">
+      <c r="W20" s="15">
         <f t="shared" si="0"/>
         <v>47157</v>
       </c>
-      <c r="X20" s="1">
+      <c r="X20" s="16">
         <f t="shared" ref="X20:X28" si="3">X19+IF(MOD(V20,4)=0,$G$10,0)</f>
         <v>0.01</v>
       </c>
     </row>
     <row r="21" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="7">
         <v>0.4375</v>
       </c>
       <c r="V21" s="1">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="W21" s="3">
+      <c r="W21" s="15">
         <f t="shared" si="0"/>
         <v>47246</v>
       </c>
-      <c r="X21" s="1">
+      <c r="X21" s="16">
         <f t="shared" si="3"/>
         <v>0.01</v>
       </c>
     </row>
     <row r="22" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="7">
         <v>0</v>
       </c>
       <c r="V22" s="1">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="W22" s="3">
+      <c r="W22" s="15">
         <f t="shared" si="0"/>
         <v>47338</v>
       </c>
-      <c r="X22" s="1">
+      <c r="X22" s="16">
         <f t="shared" si="3"/>
         <v>0.01</v>
       </c>
@@ -2051,11 +2102,11 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="W23" s="3">
+      <c r="W23" s="15">
         <f t="shared" si="0"/>
         <v>47430</v>
       </c>
-      <c r="X23" s="1">
+      <c r="X23" s="16">
         <f t="shared" si="3"/>
         <v>0.01</v>
       </c>
@@ -2065,11 +2116,11 @@
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="W24" s="3">
+      <c r="W24" s="15">
         <f t="shared" si="0"/>
         <v>47522</v>
       </c>
-      <c r="X24" s="1">
+      <c r="X24" s="16">
         <f t="shared" si="3"/>
         <v>0.01</v>
       </c>
@@ -2079,11 +2130,11 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="W25" s="3">
+      <c r="W25" s="15">
         <f t="shared" si="0"/>
         <v>47611</v>
       </c>
-      <c r="X25" s="1">
+      <c r="X25" s="16">
         <f t="shared" si="3"/>
         <v>0.01</v>
       </c>
@@ -2100,11 +2151,11 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="W26" s="3">
+      <c r="W26" s="15">
         <f t="shared" si="0"/>
         <v>47703</v>
       </c>
-      <c r="X26" s="1">
+      <c r="X26" s="16">
         <f t="shared" si="3"/>
         <v>0.01</v>
       </c>
@@ -2121,11 +2172,11 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="W27" s="3">
+      <c r="W27" s="15">
         <f t="shared" si="0"/>
         <v>47795</v>
       </c>
-      <c r="X27" s="1">
+      <c r="X27" s="16">
         <f t="shared" si="3"/>
         <v>0.01</v>
       </c>
@@ -2142,11 +2193,11 @@
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="W28" s="3">
+      <c r="W28" s="15">
         <f t="shared" si="0"/>
         <v>47889</v>
       </c>
-      <c r="X28" s="1">
+      <c r="X28" s="16">
         <f t="shared" si="3"/>
         <v>0.01</v>
       </c>
@@ -2204,10 +2255,10 @@
         <v>0</v>
       </c>
       <c r="D49" s="1">
-        <v>1000000</v>
+        <v>100000</v>
       </c>
       <c r="E49" s="1" vm="7">
-        <v>46403</v>
+        <v>45953</v>
       </c>
       <c r="F49" s="1">
         <v>180</v>
@@ -2222,19 +2273,19 @@
         <v>...</v>
       </c>
       <c r="J49" s="1">
-        <v>764898.46278708207</v>
+        <v>8023.3992552592099</v>
       </c>
       <c r="K49" s="1">
-        <v>-10879499.13942232</v>
+        <v>-12423513.905567631</v>
       </c>
       <c r="L49" s="1">
-        <v>-29806.846957321424</v>
+        <v>-34037.024398815433</v>
       </c>
       <c r="M49" s="1">
-        <v>-91384913.508427694</v>
+        <v>-86267.210155810404</v>
       </c>
       <c r="N49" s="1">
-        <v>-9138.4913508427708</v>
+        <v>-8.6267210155810403</v>
       </c>
     </row>
     <row r="50" spans="3:24" x14ac:dyDescent="0.2">
@@ -2242,10 +2293,10 @@
         <v>1</v>
       </c>
       <c r="D50" s="1">
-        <v>1000000</v>
+        <v>100000</v>
       </c>
       <c r="E50" s="1" vm="7">
-        <v>46403</v>
+        <v>45953</v>
       </c>
       <c r="F50" s="1">
         <v>180</v>
@@ -2260,19 +2311,19 @@
         <v>...</v>
       </c>
       <c r="J50" s="1">
-        <v>760828.07561082428</v>
+        <v>8020.1967944819153</v>
       </c>
       <c r="K50" s="1">
-        <v>-16110673.891427141</v>
+        <v>-13031273.298313977</v>
       </c>
       <c r="L50" s="1">
-        <v>-44138.832579252441</v>
+        <v>-35702.118625517745</v>
       </c>
       <c r="M50" s="1">
-        <v>96956978.77582176</v>
+        <v>156949.96482373824</v>
       </c>
       <c r="N50" s="1">
-        <v>9695.6978775821772</v>
+        <v>15.694996482373824</v>
       </c>
     </row>
     <row r="53" spans="3:24" x14ac:dyDescent="0.2">
@@ -2349,10 +2400,10 @@
     </row>
     <row r="57" spans="3:24" x14ac:dyDescent="0.2">
       <c r="D57" s="1">
-        <v>1000000</v>
+        <v>100000</v>
       </c>
       <c r="E57" s="1" vm="7">
-        <v>46403</v>
+        <v>45953</v>
       </c>
       <c r="F57" s="1">
         <v>180</v>
@@ -2367,7 +2418,7 @@
         <v>A</v>
       </c>
       <c r="J57" s="1">
-        <v>1.2444444444444445</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="K57" s="1" vm="9">
         <v>0</v>
@@ -2379,45 +2430,45 @@
         <v>0</v>
       </c>
       <c r="N57" s="1">
-        <v>29.871165597845863</v>
+        <v>2.3095554082585976</v>
       </c>
       <c r="O57" s="1">
-        <v>-0.36994905378514381</v>
+        <v>-0.35305563284214747</v>
       </c>
       <c r="P57" s="1">
-        <v>29871165.597845864</v>
+        <v>230955.54082585976</v>
       </c>
       <c r="Q57" s="1">
-        <v>-369949.05378514383</v>
+        <v>-35305.563284214746</v>
       </c>
       <c r="R57" s="1">
-        <v>4448.8290148558272</v>
+        <v>3938.8817428978164</v>
       </c>
       <c r="S57" s="1">
-        <v>76489846.278708205</v>
+        <v>802339.92552592105</v>
       </c>
       <c r="T57" s="1">
-        <v>764898.46278708207</v>
+        <v>8023.3992552592099</v>
       </c>
       <c r="U57" s="1">
-        <v>-10879499.13942232</v>
+        <v>-12423513.905567631</v>
       </c>
       <c r="V57" s="1">
-        <v>-29806.846957321424</v>
+        <v>-34037.024398815433</v>
       </c>
       <c r="W57" s="1">
-        <v>-91384913.508427694</v>
+        <v>-86267.210155810404</v>
       </c>
       <c r="X57" s="1">
-        <v>-9138.4913508427708</v>
+        <v>-8.6267210155810403</v>
       </c>
     </row>
     <row r="58" spans="3:24" x14ac:dyDescent="0.2">
       <c r="D58" s="1">
-        <v>1000000</v>
+        <v>100000</v>
       </c>
       <c r="E58" s="1" vm="7">
-        <v>46403</v>
+        <v>45953</v>
       </c>
       <c r="F58" s="1">
         <v>180</v>
@@ -2432,7 +2483,7 @@
         <v>A</v>
       </c>
       <c r="J58" s="1">
-        <v>1.2444444444444445</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="K58" s="1" vm="9">
         <v>0</v>
@@ -2444,37 +2495,37 @@
         <v>0</v>
       </c>
       <c r="N58" s="1">
-        <v>39.952099164325155</v>
+        <v>5.6151629774481515</v>
       </c>
       <c r="O58" s="1">
-        <v>0.64378101699318313</v>
+        <v>0.64733544856512815</v>
       </c>
       <c r="P58" s="1">
-        <v>39952099.164325155</v>
+        <v>561516.29774481512</v>
       </c>
       <c r="Q58" s="1">
-        <v>643781.01699318318</v>
+        <v>64733.544856512817</v>
       </c>
       <c r="R58" s="1">
-        <v>4163.3692204800382</v>
+        <v>3931.9723866686077</v>
       </c>
       <c r="S58" s="1">
-        <v>76082807.561082438</v>
+        <v>802019.67944819154</v>
       </c>
       <c r="T58" s="1">
-        <v>760828.07561082428</v>
+        <v>8020.1967944819153</v>
       </c>
       <c r="U58" s="1">
-        <v>-16110673.891427141</v>
+        <v>-13031273.298313977</v>
       </c>
       <c r="V58" s="1">
-        <v>-44138.832579252441</v>
+        <v>-35702.118625517745</v>
       </c>
       <c r="W58" s="1">
-        <v>96956978.77582176</v>
+        <v>156949.96482373824</v>
       </c>
       <c r="X58" s="1">
-        <v>9695.6978775821772</v>
+        <v>15.694996482373824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>